<commit_message>
Se actualizaron archivos de Medidas 1 , codigo Arduino
</commit_message>
<xml_diff>
--- a/Medidas Electronicas I/Mediciones 1er Trabajo Regresion lineal.xlsx
+++ b/Medidas Electronicas I/Mediciones 1er Trabajo Regresion lineal.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="7">
-  <si>
-    <t>Corriente</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="7">
   <si>
     <t>Tension</t>
   </si>
@@ -38,16 +35,20 @@
   <si>
     <t>Promedio</t>
   </si>
+  <si>
+    <t>Corriente mA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
-    <numFmt numFmtId="165" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -78,11 +79,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -129,17 +131,35 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:trendline>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.44979986876640421"/>
+                  <c:y val="-5.5371463983668705E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$C$3:$C$12</c:f>
+              <c:f>Hoja1!$K$3:$K$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>99.18</c:v>
                 </c:pt>
@@ -169,16 +189,55 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>98.97</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1005</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3009</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3009</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3009</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$3:$D$12</c:f>
+              <c:f>Hoja1!$L$3:$L$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>2.5129999999999999</c:v>
                 </c:pt>
@@ -208,6 +267,45 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2.5129999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.589</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.589</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.589</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.589</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.6760000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.677</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.677</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.677</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.677</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.0590000000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.0590000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -222,11 +320,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65523072"/>
-        <c:axId val="65521536"/>
+        <c:axId val="72555904"/>
+        <c:axId val="72553984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65523072"/>
+        <c:axId val="72555904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -236,12 +334,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65521536"/>
+        <c:crossAx val="72553984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65521536"/>
+        <c:axId val="72553984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -252,150 +350,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65523072"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Hoja1!$C$28:$C$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>3046</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3009</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3009</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3009</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3008</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Hoja1!$D$28:$D$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>3.0550000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.06</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0590000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.06</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.0590000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="111043712"/>
-        <c:axId val="111032192"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="111043712"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111032192"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="111032192"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111043712"/>
+        <c:crossAx val="72555904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -421,20 +376,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="1 Gráfico"/>
+        <xdr:cNvPr id="6" name="5 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -444,36 +399,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="3 Gráfico"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -769,28 +694,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G32"/>
+  <dimension ref="B2:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>2</v>
       </c>
       <c r="C3" s="3">
         <v>99.18</v>
@@ -799,12 +733,18 @@
         <v>2.5129999999999999</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>99.18</v>
+      </c>
+      <c r="L3" s="3">
+        <v>2.5129999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
         <v>99</v>
@@ -820,10 +760,16 @@
         <f>AVERAGE(D3:D12)</f>
         <v>2.5129999999999995</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K4" s="3">
+        <v>99</v>
+      </c>
+      <c r="L4" s="3">
+        <v>2.5129999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3">
         <v>98.9</v>
@@ -831,10 +777,16 @@
       <c r="D5" s="3">
         <v>2.5129999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K5" s="3">
+        <v>98.9</v>
+      </c>
+      <c r="L5" s="3">
+        <v>2.5129999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
         <v>98.92</v>
@@ -842,10 +794,16 @@
       <c r="D6" s="3">
         <v>2.5129999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K6" s="3">
+        <v>98.92</v>
+      </c>
+      <c r="L6" s="3">
+        <v>2.5129999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3">
         <v>98.99</v>
@@ -853,10 +811,16 @@
       <c r="D7" s="3">
         <v>2.5129999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K7" s="3">
+        <v>98.99</v>
+      </c>
+      <c r="L7" s="3">
+        <v>2.5129999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3">
         <v>98.98</v>
@@ -864,10 +828,16 @@
       <c r="D8" s="3">
         <v>2.5129999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K8" s="3">
+        <v>98.98</v>
+      </c>
+      <c r="L8" s="3">
+        <v>2.5129999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3">
         <v>98.91</v>
@@ -875,10 +845,16 @@
       <c r="D9" s="3">
         <v>2.5129999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K9" s="3">
+        <v>98.91</v>
+      </c>
+      <c r="L9" s="3">
+        <v>2.5129999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
         <v>98.99</v>
@@ -886,10 +862,16 @@
       <c r="D10" s="3">
         <v>2.5129999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K10" s="3">
+        <v>98.99</v>
+      </c>
+      <c r="L10" s="3">
+        <v>2.5129999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="3">
         <v>98.95</v>
@@ -897,10 +879,16 @@
       <c r="D11" s="3">
         <v>2.5129999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K11" s="3">
+        <v>98.95</v>
+      </c>
+      <c r="L11" s="3">
+        <v>2.5129999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="3">
         <v>98.97</v>
@@ -908,18 +896,38 @@
       <c r="D12" s="3">
         <v>2.5129999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="K12" s="3">
+        <v>98.97</v>
+      </c>
+      <c r="L12" s="3">
+        <v>2.5129999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K13" s="3">
+        <v>505</v>
+      </c>
+      <c r="L13" s="3">
+        <v>2.589</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
         <v>0</v>
       </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K14" s="3">
+        <v>505</v>
+      </c>
+      <c r="L14" s="3">
+        <v>2.589</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="3">
         <v>505</v>
@@ -928,12 +936,18 @@
         <v>2.589</v>
       </c>
       <c r="F15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="K15" s="3">
+        <v>505</v>
+      </c>
+      <c r="L15" s="3">
+        <v>2.589</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" s="3">
         <v>505</v>
@@ -949,10 +963,16 @@
         <f>AVERAGE(D15:D18)</f>
         <v>2.589</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K16" s="3">
+        <v>505</v>
+      </c>
+      <c r="L16" s="3">
+        <v>2.589</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" s="3">
         <v>505</v>
@@ -960,10 +980,16 @@
       <c r="D17" s="3">
         <v>2.589</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K17" s="3">
+        <v>1005</v>
+      </c>
+      <c r="L17" s="3">
+        <v>2.6760000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" s="3">
         <v>505</v>
@@ -971,21 +997,39 @@
       <c r="D18" s="3">
         <v>2.589</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K18" s="3">
+        <v>1005</v>
+      </c>
+      <c r="L18" s="3">
+        <v>2.677</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="K19" s="3">
+        <v>1005</v>
+      </c>
+      <c r="L19" s="3">
+        <v>2.677</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
         <v>0</v>
       </c>
-      <c r="C20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K20" s="3">
+        <v>1005</v>
+      </c>
+      <c r="L20" s="3">
+        <v>2.677</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" s="3">
         <v>1005</v>
@@ -994,12 +1038,25 @@
         <v>2.6760000000000002</v>
       </c>
       <c r="F21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="K21" s="3">
+        <v>1004</v>
+      </c>
+      <c r="L21" s="3">
+        <v>2.677</v>
+      </c>
+      <c r="N21" s="8">
+        <f t="array" ref="N21:O24">LINEST(L3:L25,K3:K25,TRUE,TRUE)</f>
+        <v>1.8766241153689634E-4</v>
+      </c>
+      <c r="O21" s="8">
+        <v>2.4931235857379326</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="3">
         <v>1005</v>
@@ -1015,10 +1072,22 @@
         <f>AVERAGE(D21:D25)</f>
         <v>2.6767999999999996</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K22" s="3">
+        <v>3009</v>
+      </c>
+      <c r="L22" s="3">
+        <v>3.06</v>
+      </c>
+      <c r="N22" s="8">
+        <v>5.4518567392640364E-7</v>
+      </c>
+      <c r="O22" s="8">
+        <v>7.4001924744230099E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23" s="3">
         <v>1005</v>
@@ -1026,10 +1095,22 @@
       <c r="D23" s="3">
         <v>2.677</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K23" s="3">
+        <v>3009</v>
+      </c>
+      <c r="L23" s="3">
+        <v>3.0590000000000002</v>
+      </c>
+      <c r="N23" s="8">
+        <v>0.99982279473825253</v>
+      </c>
+      <c r="O23" s="8">
+        <v>2.71857734787083E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24" s="3">
         <v>1005</v>
@@ -1037,10 +1118,22 @@
       <c r="D24" s="3">
         <v>2.677</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K24" s="3">
+        <v>3009</v>
+      </c>
+      <c r="L24" s="3">
+        <v>3.06</v>
+      </c>
+      <c r="N24" s="8">
+        <v>118485.63909702984</v>
+      </c>
+      <c r="O24" s="8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25" s="3">
         <v>1004</v>
@@ -1048,18 +1141,24 @@
       <c r="D25" s="3">
         <v>2.677</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="K25" s="3">
+        <v>3008</v>
+      </c>
+      <c r="L25" s="3">
+        <v>3.0590000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
         <v>0</v>
       </c>
-      <c r="C27" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="3">
         <v>3046</v>
@@ -1068,12 +1167,12 @@
         <v>3.0550000000000002</v>
       </c>
       <c r="F28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="3">
         <v>3009</v>
@@ -1090,9 +1189,9 @@
         <v>3.0585999999999998</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="3">
         <v>3009</v>
@@ -1101,9 +1200,9 @@
         <v>3.0590000000000002</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="3">
         <v>3009</v>
@@ -1112,9 +1211,9 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" s="3">
         <v>3008</v>

</xml_diff>